<commit_message>
update image list , to print word and number
</commit_message>
<xml_diff>
--- a/doc/Surg_class.xlsx
+++ b/doc/Surg_class.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -991,36 +991,36 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cancer of the testis most likely metastases to which set of lymph nodes?</t>
+          <t>A 28-year-old female figure skater presents several weeks after having sustained an injury to her left breast. She has a painful mass shown in the upper outer quadrant. Skin retraction is noticed, and a hard mass, 3–4 cm in diameter, can easily be palpated. What is the most likely diagnosis?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Aortic.</t>
+          <t>Infiltrating carcinoma.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Deep inguinal.</t>
+          <t>Breast abscess.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Superficial inguinal.</t>
+          <t>Hematoma.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Common iliac.</t>
+          <t>Fat necrosis.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Internal iliac.</t>
+          <t>Sclerosing adenosis.</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1031,36 +1031,36 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A 57-year-old man is brought to the emergency department complaining of dyspnea and chest pain. He also admits to a 20-lb weight loss. He complains of fevers, chills, and night sweats. Physical examination reveals supraclavicular adenopathy. Chest examination reveals distant heart sounds. Laboratory studies reveal a white blood cell count of 170,000/mL. Chest x-ray and echocardiography revealed a pericardial effusion. What is the most likely explanation for these findings?</t>
+          <t>Cancer of the testis most likely metastases to which set of lymph nodes?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Atrial myxoma.</t>
+          <t>Aortic.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Atrial fibrillation.</t>
+          <t>Deep inguinal.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Lymphoma.</t>
+          <t>Superficial inguinal.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Metastatic colorectal carcinoma.</t>
+          <t>Common iliac.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Pericarditis.</t>
+          <t>Internal iliac.</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1071,36 +1071,36 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>A 40-year-old woman undergoes repair of a right femoral hernia. During the procedure, the femoral canal is dissected. The anatomic boundaries of the femoral canal include which of the following?</t>
+          <t>A 57-year-old man is brought to the emergency department complaining of dyspnea and chest pain. He also admits to a 20-lb weight loss. He complains of fevers, chills, and night sweats. Physical examination reveals supraclavicular adenopathy. Chest examination reveals distant heart sounds. Laboratory studies reveal a white blood cell count of 170,000/mL. Chest x-ray and echocardiography revealed a pericardial effusion. What is the most likely explanation for these findings?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cooper ligament.</t>
+          <t>Atrial myxoma.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Inguinal ligament.</t>
+          <t>Atrial fibrillation.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Ischial spine.</t>
+          <t>Lymphoma.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Lacunar ligament.</t>
+          <t>Metastatic colorectal carcinoma.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Nerve (femoral).</t>
+          <t>Pericarditis.</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1111,36 +1111,36 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A 39-year-old woman presents to the emergency department complaining of severe abdominal pain. She has a history of peptic ulcer disease. Physical examination reveals guarding and rebound tenderness. She is taken to the operating room for exploratory laparotomy. During the procedure, the surgeon who opens the gastrosplenic ligament to reach the lesser sac accidentally cuts an artery. Which of the following vessels is the most likely one injured?</t>
+          <t>A 40-year-old woman undergoes repair of a right femoral hernia. During the procedure, the femoral canal is dissected. The anatomic boundaries of the femoral canal include which of the following?</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Gastroduodenal artery.</t>
+          <t>Cooper ligament.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Left gastric artery.</t>
+          <t>Inguinal ligament.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Left gastroepiploic artery.</t>
+          <t>Ischial spine.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Right gastric artery.</t>
+          <t>Lacunar ligament.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Splenic artery.</t>
+          <t>Nerve (femoral).</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1151,32 +1151,32 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A 12-year-old boy is brought to his physician for evaluation of a neck mass. He has a history of recurrent sinusitis and tonsillar infections. Physical examination reveals a midline neck mass measuring 1.5 cm that moves with swallowing. There is no evidence of lymphadenopathy. What is the most likely diagnosis?</t>
+          <t>A 39-year-old woman presents to the emergency department complaining of severe abdominal pain. She has a history of peptic ulcer disease. Physical examination reveals guarding and rebound tenderness. She is taken to the operating room for exploratory laparotomy. During the procedure, the surgeon who opens the gastrosplenic ligament to reach the lesser sac accidentally cuts an artery. Which of the following vessels is the most likely one injured?</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Leukemia.</t>
+          <t>Gastroduodenal artery.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Lymphoma.</t>
+          <t>Left gastric artery.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Thyroglossal duct cyst.</t>
+          <t>Left gastroepiploic artery.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Thyroglossal fistula.</t>
+          <t>Right gastric artery.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Thyroid carcinoma.</t>
+          <t>Splenic artery.</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1191,27 +1191,32 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The three findings in achalasia are:</t>
+          <t>A 12-year-old boy is brought to his physician for evaluation of a neck mass. He has a history of recurrent sinusitis and tonsillar infections. Physical examination reveals a midline neck mass measuring 1.5 cm that moves with swallowing. There is no evidence of lymphadenopathy. What is the most likely diagnosis?</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Increased LES resting pressure, decreased LES relaxation, increased esophageal peristaltic activity.</t>
+          <t>Leukemia.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Decreased LES resting pressure, increased LES relaxation, decreased esophageal peristaltic activity.</t>
+          <t>Lymphoma.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Increased LES resting pressure, decreased LES relaxation, decreased esophageal peristaltic activity.</t>
+          <t>Thyroglossal duct cyst.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Decreased LES resting pressure, increased LES relaxation, increased esophageal peristaltic activity.</t>
+          <t>Thyroglossal fistula.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Thyroid carcinoma.</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1226,31 +1231,31 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A 70-kg male patient presents to ED following a stab wound to the abdomen. He is hypotensive, markedly tachycardic (145 beats/min), and appears confused. What percent of blood volume has he lost?</t>
+          <t>The three findings in achalasia are:</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5%.</t>
+          <t>Increased LES resting pressure, decreased LES relaxation, increased esophageal peristaltic activity.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>15%.</t>
+          <t>Decreased LES resting pressure, increased LES relaxation, decreased esophageal peristaltic activity.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>35%.</t>
+          <t>Increased LES resting pressure, decreased LES relaxation, decreased esophageal peristaltic activity.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>55%.</t>
+          <t>Decreased LES resting pressure, increased LES relaxation, increased esophageal peristaltic activity.</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -1261,31 +1266,31 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Neurogenic shock is characterized by the presence of</t>
+          <t>A 70-kg male patient presents to ED following a stab wound to the abdomen. He is hypotensive, markedly tachycardic (145 beats/min), and appears confused. What percent of blood volume has he lost?</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Cool, moist skin.</t>
+          <t>5%.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Increased cardiac output.</t>
+          <t>15%.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Decreased peripheral vascular resistance.</t>
+          <t>35%.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Decreased blood volume.</t>
+          <t>55%.</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
@@ -1296,31 +1301,31 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The shock caused by a large tension pneumothorax is categorized as</t>
+          <t>Neurogenic shock is characterized by the presence of</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Trauma shock.</t>
+          <t>Cool, moist skin.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Vasodilatory shock.</t>
+          <t>Increased cardiac output.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Cardiogenic shock.</t>
+          <t>Decreased peripheral vascular resistance.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Obstructive shock.</t>
+          <t>Decreased blood volume.</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1331,36 +1336,31 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Calcitonin is used as a tumor marker for which of the following thyroid tumors:</t>
+          <t>The shock caused by a large tension pneumothorax is categorized as</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Anaplastic thyroid ca.</t>
+          <t>Trauma shock.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Follicular thyroid ca.</t>
+          <t>Vasodilatory shock.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Papillary thyroid ca.</t>
+          <t>Cardiogenic shock.</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Lymphoma of the thyroid.</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Medullary thyroid carcinoma.</t>
+          <t>Obstructive shock.</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1371,36 +1371,36 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Which of the following fluid compartments contains the largest volume?</t>
+          <t>Calcitonin is used as a tumor marker for which of the following thyroid tumors:</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>plasma.</t>
+          <t>Anaplastic thyroid ca.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>interstitial compartment.</t>
+          <t>Follicular thyroid ca.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>intracellular compartment.</t>
+          <t>Papillary thyroid ca.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>extracellular compartment.</t>
+          <t>Lymphoma of the thyroid.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>lymph.</t>
+          <t>Medullary thyroid carcinoma.</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1411,36 +1411,36 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The predominant intracellular cation is</t>
+          <t>Which of the following fluid compartments contains the largest volume?</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>potassium.</t>
+          <t>plasma.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>sodium.</t>
+          <t>interstitial compartment.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>calcium.</t>
+          <t>intracellular compartment.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>magnesium.</t>
+          <t>extracellular compartment.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>chloride.</t>
+          <t>lymph.</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1451,36 +1451,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Receptors sensitive to changes in the osmolality of extracellular fluid are the</t>
+          <t>The predominant intracellular cation is</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>baroreceptors.</t>
+          <t>potassium.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>chemoreceptors.</t>
+          <t>sodium.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>osmoreceptors.</t>
+          <t>calcium.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>pressoreceptors.</t>
+          <t>magnesium.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>proprioreceptors.</t>
+          <t>chloride.</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1491,36 +1491,36 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Renin is released by the</t>
+          <t>Receptors sensitive to changes in the osmolality of extracellular fluid are the</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>lungs.</t>
+          <t>baroreceptors.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>kidney.</t>
+          <t>chemoreceptors.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>spleen.</t>
+          <t>osmoreceptors.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>liver.</t>
+          <t>pressoreceptors.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>pancreas.</t>
+          <t>proprioreceptors.</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1531,36 +1531,36 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Visceral pain is typically:</t>
+          <t>Renin is released by the</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Well localized.</t>
+          <t>lungs.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sharp.</t>
+          <t>kidney.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Mediated via spinal nerves.</t>
+          <t>spleen.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Perceived to be in the midline.</t>
+          <t>liver.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Perceived to be in the loin.</t>
+          <t>pancreas.</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1571,32 +1571,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A 30-year-old restrained driver was involved in a motor vehicle crash. He is hemodynamically stable and has a large seat belt sign on the abdomen. His abdomen is tender to palpation. In this patient one should be most concerned about:</t>
+          <t>Visceral pain is typically:</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Liver and spleen injury.</t>
+          <t>Well localized.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Transection of the head of the pancreas.</t>
+          <t>Sharp.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Renal pedicle avulsion.</t>
+          <t>Mediated via spinal nerves.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Hollow-viscus injuries.</t>
+          <t>Perceived to be in the midline.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Pelvic fracture.</t>
+          <t>Perceived to be in the loin.</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -1611,32 +1611,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The characteristic changes that follow a major operation or moderate to severe injury do not include the following:</t>
+          <t>A 30-year-old restrained driver was involved in a motor vehicle crash. He is hemodynamically stable and has a large seat belt sign on the abdomen. His abdomen is tender to palpation. In this patient one should be most concerned about:</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Hypermetabolism.</t>
+          <t>Liver and spleen injury.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Fever.</t>
+          <t>Transection of the head of the pancreas.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Tachypnea.</t>
+          <t>Renal pedicle avulsion.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Hyperphagia.</t>
+          <t>Hollow-viscus injuries.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Negative nitrogen balance.</t>
+          <t>Pelvic fracture.</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -1651,36 +1651,36 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Scar formation is part of the normal healing process following injury. Which of the following tissues has the ability to heal without scar formation?</t>
+          <t>The characteristic changes that follow a major operation or moderate to severe injury do not include the following:</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Liver.</t>
+          <t>Hypermetabolism.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Skin.</t>
+          <t>Fever.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Bone.</t>
+          <t>Tachypnea.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Muscle.</t>
+          <t>Hyperphagia.</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Nerves.</t>
+          <t>Negative nitrogen balance.</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1691,36 +1691,36 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>There are a number of hypercoagulable states which can be associated with arterial or venous thrombosis and embolic phenomenon. These include:</t>
+          <t>Scar formation is part of the normal healing process following injury. Which of the following tissues has the ability to heal without scar formation?</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Heparin-associated thrombocytosis.</t>
+          <t>Liver.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Antithrombin III deficiency.</t>
+          <t>Skin.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Von Willebrand disease.</t>
+          <t>Bone.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Vitamin C deficiency.</t>
+          <t>Muscle.</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>None of above.</t>
+          <t>Nerves.</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -1731,36 +1731,36 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>An 11-year-old boy has experienced severe diarrhea for 10 days. He presents with decreased skin turgor, sunken eyes, orthostatic hypotension, and tachycardia. Which of the following statement may be true concerning his diagnosis and treatment?</t>
+          <t>There are a number of hypercoagulable states which can be associated with arterial or venous thrombosis and embolic phenomenon. These include:</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>His hematocrit will likely be elevated.</t>
+          <t>Heparin-associated thrombocytosis.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>His BUN may be elevated in proportion to serum creatinine.</t>
+          <t>Antithrombin III deficiency.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>His serum sodium will be elevated.</t>
+          <t>Von Willebrand disease.</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Fluid resuscitation should begin with D5 1/2 normal saline because of the expected high serum sodium associated with excessive fluid loss.</t>
+          <t>Vitamin C deficiency.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>All of the above.</t>
+          <t>None of above.</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1771,36 +1771,36 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nasotracheal intubation:</t>
+          <t>An 11-year-old boy has experienced severe diarrhea for 10 days. He presents with decreased skin turgor, sunken eyes, orthostatic hypotension, and tachycardia. Which of the following statement may be true concerning his diagnosis and treatment?</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Is preferred for the unconscious patient without a cervical spine injury.</t>
+          <t>His hematocrit will likely be elevated.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Is preferred for patients with a suspected cervical spine injury.</t>
+          <t>His BUN may be elevated in proportion to serum creatinine.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Maximizes neck manipulation.</t>
+          <t>His serum sodium will be elevated.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Is contraindicated in the patient who is breathing spontaneously.</t>
+          <t>Fluid resuscitation should begin with D5 1/2 normal saline because of the expected high serum sodium associated with excessive fluid loss.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Had no rule in trauma.</t>
+          <t>All of the above.</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1811,36 +1811,36 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The hypermetabolic response seen in patients with large burns, who are successfully resuscitated, is thought to be driven by which of the following factors?</t>
+          <t>Nasotracheal intubation:</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Deficient gastrointestinal barrier function.</t>
+          <t>Is preferred for the unconscious patient without a cervical spine injury.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Bacterial contamination of the burn wound.</t>
+          <t>Is preferred for patients with a suspected cervical spine injury.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Evaporative heat loss.</t>
+          <t>Maximizes neck manipulation.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Changes in hypothalamic function.</t>
+          <t>Is contraindicated in the patient who is breathing spontaneously.</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>All of the above.</t>
+          <t>Had no rule in trauma.</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1851,36 +1851,36 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Worldwide, the most important predisposing factor for hepatocellular carcinoma (HCC) is:</t>
+          <t>The hypermetabolic response seen in patients with large burns, who are successfully resuscitated, is thought to be driven by which of the following factors?</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Alcoholic cirrhosis.</t>
+          <t>Deficient gastrointestinal barrier function.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Hepatitis B infection.</t>
+          <t>Bacterial contamination of the burn wound.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Chronic liver disease of any etiology.</t>
+          <t>Evaporative heat loss.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Hepatitis C infection.</t>
+          <t>Changes in hypothalamic function.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Repeated ingestion of Aflatoxin.</t>
+          <t>All of the above.</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1891,36 +1891,36 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>About Hereditary spherocytosis (HS), one of the following is TRUE:</t>
+          <t>Worldwide, the most important predisposing factor for hepatocellular carcinoma (HCC) is:</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>It is an autosomal recessive hereditary disorder.</t>
+          <t>Alcoholic cirrhosis.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>It is associated with gallstones at an early age.</t>
+          <t>Hepatitis B infection.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>There is a decrease in the permeability of the red cell membranes to sodium.</t>
+          <t>Chronic liver disease of any etiology.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>The fragility test is usually negative.</t>
+          <t>Hepatitis C infection.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Splenectomy is rarely indicated.</t>
+          <t>Repeated ingestion of Aflatoxin.</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1931,36 +1931,36 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>An 18-year-old woman at 9 weeks gestation is brought to the emergency department because of an open fracture of the tibia and fibula. She is hemodynamically stabilized and referred to the orthopedic department. She is scheduled for internal fixation of the tibia the following day. However, before the surgery she develops severe dyspnea and confusion. Her temperature is 37. C, blood pressure is 110/70 mm Hg, pulse is 110 /min, and respirations are 22/min. Examination shows numerous non-palpable petechiae in the upper part of the body. Which of the following is the most likely diagnosis?</t>
+          <t>About Hereditary spherocytosis (HS), one of the following is TRUE:</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Air embolism.</t>
+          <t>It is an autosomal recessive hereditary disorder.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Amniotic fluid embolism.</t>
+          <t>It is associated with gallstones at an early age.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Thromboembolism.</t>
+          <t>There is a decrease in the permeability of the red cell membranes to sodium.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Fat embolism.</t>
+          <t>The fragility test is usually negative.</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Acute respiratory distress syndrome.</t>
+          <t>Splenectomy is rarely indicated.</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1971,35 +1971,75 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>An 18-year-old woman at 9 weeks gestation is brought to the emergency department because of an open fracture of the tibia and fibula. She is hemodynamically stabilized and referred to the orthopedic department. She is scheduled for internal fixation of the tibia the following day. However, before the surgery she develops severe dyspnea and confusion. Her temperature is 37. C, blood pressure is 110/70 mm Hg, pulse is 110 /min, and respirations are 22/min. Examination shows numerous non-palpable petechiae in the upper part of the body. Which of the following is the most likely diagnosis?</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Air embolism.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Amniotic fluid embolism.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Thromboembolism.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Fat embolism.</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Acute respiratory distress syndrome.</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>mc</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>A 40- year-old female is brought to the emergency department following a motor vehicle accident in which she was the front seat passenger. Examination of the right leg reveals a hematoma over the thigh. Knee extension on the right is markedly reduced when compared to the left. Sensory examination reveals decreased sensory perception of both sharp and dull stimuli over the medial side of the right lower thigh and leg. All other dermatomes are intact. What nerve injury is most likely present in this patient?</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>Femoral nerve.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Tibial nerve.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>Obturator nerve.</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>Common peroneal nerve.</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>Fibular nerve.</t>
         </is>
       </c>
-      <c r="H40" t="n">
+      <c r="H41" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>